<commit_message>
move to association class, fixing JPA duplicates
</commit_message>
<xml_diff>
--- a/owlcms/local/agegroups/AgeGroups_Dev.xlsx
+++ b/owlcms/local/agegroups/AgeGroups_Dev.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms4\owlcms\local\agegroups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD17FC84-3AD3-41E5-A9E8-8F289B306E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BE1ED3E-8AC7-429F-9FF7-38A8366683EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5265" yWindow="1200" windowWidth="21600" windowHeight="11205" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BW Categories" sheetId="1" r:id="rId1"/>
@@ -1076,8 +1076,8 @@
   </sheetPr>
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2073,7 +2073,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="1" t="s">
@@ -2128,7 +2128,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="1"/>
@@ -2183,7 +2183,7 @@
         <v>999</v>
       </c>
       <c r="G21" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="1"/>
@@ -2238,7 +2238,7 @@
         <v>999</v>
       </c>
       <c r="G22" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>29</v>
@@ -3173,7 +3173,7 @@
         <v>17</v>
       </c>
       <c r="G39" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -3228,7 +3228,7 @@
         <v>20</v>
       </c>
       <c r="G40" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -3283,7 +3283,7 @@
         <v>999</v>
       </c>
       <c r="G41" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -3338,7 +3338,7 @@
         <v>999</v>
       </c>
       <c r="G42" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>11</v>

</xml_diff>